<commit_message>
Added GPU parallel computing
</commit_message>
<xml_diff>
--- a/untested.xlsx
+++ b/untested.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\duter\Documents\JHU MSIS\Managing Complex Projects\Simulation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\duter\Documents\JHU MSIS\Managing Complex Projects\ArtificialStupidity_Harvard_PM_Sim\ArtificialStupidity_Harvard_PM_Sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE9A4D6-9652-4A91-A0C7-480D675F45F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB5544D-40DC-40D4-A44F-45AC63BFE830}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34395" yWindow="0" windowWidth="17205" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45030" yWindow="3075" windowWidth="16905" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -185,8 +185,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E755F329-7319-4CF3-A9A9-DEC1F7819412}" name="Table1" displayName="Table1" ref="A1:O80" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:O80" xr:uid="{CAC85D1A-9F60-44BF-A6C0-744D6342ABB0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E755F329-7319-4CF3-A9A9-DEC1F7819412}" name="Table1" displayName="Table1" ref="A1:O77" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:O77" xr:uid="{CAC85D1A-9F60-44BF-A6C0-744D6342ABB0}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{DC50FC25-2696-4618-A657-38949E25B5BD}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{2C0C76A9-780E-4829-A93F-10DFED91771C}" name="Weeks"/>
@@ -495,16 +495,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O80"/>
+  <dimension ref="A1:O77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
     <col min="3" max="3" width="8.140625" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
     <col min="5" max="5" width="4.140625" customWidth="1"/>
@@ -608,7 +608,7 @@
         <v>14</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O45" si="0">A2</f>
+        <f t="shared" ref="O2:O43" si="0">A2</f>
         <v>0</v>
       </c>
     </row>
@@ -1109,16 +1109,16 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1127,13 +1127,13 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14">
         <v>25</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O14">
         <f t="shared" si="0"/>
@@ -1154,43 +1154,43 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I15">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O15">
         <f t="shared" si="0"/>
@@ -1199,22 +1199,22 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -1226,16 +1226,16 @@
         <v>3</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O16">
         <f t="shared" si="0"/>
@@ -1244,43 +1244,43 @@
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="O17">
         <f t="shared" si="0"/>
@@ -1289,43 +1289,43 @@
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>20</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
         <v>7</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>25</v>
-      </c>
-      <c r="J18">
-        <v>3</v>
-      </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
       </c>
       <c r="O18">
         <f t="shared" si="0"/>
@@ -1334,43 +1334,43 @@
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I19">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
       <c r="N19">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="O19">
         <f t="shared" si="0"/>
@@ -1379,31 +1379,31 @@
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>2</v>
       </c>
       <c r="I20">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -1415,7 +1415,7 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="O20">
         <f t="shared" si="0"/>
@@ -1424,43 +1424,43 @@
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="I21">
         <v>10</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>3</v>
-      </c>
-      <c r="I21">
-        <v>20</v>
-      </c>
       <c r="J21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O21">
         <f t="shared" si="0"/>
@@ -1469,43 +1469,43 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C22">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
         <v>10</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>2</v>
-      </c>
-      <c r="I22">
-        <v>15</v>
-      </c>
       <c r="J22">
         <v>1</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="O22">
         <f t="shared" si="0"/>
@@ -1514,16 +1514,16 @@
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C23">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1550,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="N23">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O23">
         <f t="shared" si="0"/>
@@ -1559,10 +1559,10 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C24">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1571,31 +1571,31 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24">
         <v>1</v>
       </c>
       <c r="I24">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
       <c r="N24">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="O24">
         <f t="shared" si="0"/>
@@ -1604,13 +1604,13 @@
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1619,28 +1619,28 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25">
         <v>0</v>
       </c>
       <c r="N25">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O25">
         <f t="shared" si="0"/>
@@ -1649,19 +1649,19 @@
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1670,22 +1670,22 @@
         <v>1</v>
       </c>
       <c r="I26">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26">
         <v>0</v>
       </c>
       <c r="N26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O26">
         <f t="shared" si="0"/>
@@ -1697,7 +1697,7 @@
         <v>7</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -1706,31 +1706,31 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
       <c r="I27">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J27">
         <v>2</v>
       </c>
       <c r="K27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
       <c r="N27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O27">
         <f t="shared" si="0"/>
@@ -1739,10 +1739,10 @@
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -1757,10 +1757,10 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I28">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="J28">
         <v>3</v>
@@ -1775,7 +1775,7 @@
         <v>0</v>
       </c>
       <c r="N28">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O28">
         <f t="shared" si="0"/>
@@ -1784,10 +1784,10 @@
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1796,19 +1796,19 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I29">
         <v>5</v>
       </c>
       <c r="J29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -1820,7 +1820,7 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="O29">
         <f t="shared" si="0"/>
@@ -1829,31 +1829,31 @@
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C30">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I30">
         <v>25</v>
       </c>
       <c r="J30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -1865,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="N30">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O30">
         <f t="shared" si="0"/>
@@ -1874,43 +1874,43 @@
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C31">
+        <v>9</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>3</v>
+      </c>
+      <c r="I31">
+        <v>15</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
         <v>12</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <v>2</v>
-      </c>
-      <c r="I31">
-        <v>5</v>
-      </c>
-      <c r="J31">
-        <v>3</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>1</v>
-      </c>
-      <c r="M31">
-        <v>0</v>
-      </c>
-      <c r="N31">
-        <v>18</v>
       </c>
       <c r="O31">
         <f t="shared" si="0"/>
@@ -1919,10 +1919,10 @@
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C32">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1931,31 +1931,31 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
       <c r="I32">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32">
         <v>0</v>
       </c>
       <c r="N32">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="O32">
         <f t="shared" si="0"/>
@@ -1964,13 +1964,13 @@
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C33">
         <v>9</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1979,28 +1979,28 @@
         <v>0</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33">
         <v>3</v>
       </c>
       <c r="I33">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J33">
         <v>1</v>
       </c>
       <c r="K33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33">
         <v>0</v>
       </c>
       <c r="N33">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="O33">
         <f t="shared" si="0"/>
@@ -2009,13 +2009,13 @@
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C34">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -2024,28 +2024,28 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I34">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34">
         <v>0</v>
       </c>
       <c r="N34">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O34">
         <f t="shared" si="0"/>
@@ -2054,13 +2054,13 @@
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C35">
         <v>9</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -2069,13 +2069,13 @@
         <v>0</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I35">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J35">
         <v>1</v>
@@ -2090,7 +2090,7 @@
         <v>0</v>
       </c>
       <c r="N35">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="O35">
         <f t="shared" si="0"/>
@@ -2102,7 +2102,7 @@
         <v>8</v>
       </c>
       <c r="C36">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -2123,19 +2123,19 @@
         <v>15</v>
       </c>
       <c r="J36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M36">
         <v>0</v>
       </c>
       <c r="N36">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O36">
         <f t="shared" si="0"/>
@@ -2144,10 +2144,10 @@
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C37">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -2165,22 +2165,22 @@
         <v>1</v>
       </c>
       <c r="I37">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37">
         <v>0</v>
       </c>
       <c r="N37">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O37">
         <f t="shared" si="0"/>
@@ -2189,13 +2189,13 @@
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C38">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -2204,16 +2204,16 @@
         <v>0</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I38">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K38">
         <v>0</v>
@@ -2225,7 +2225,7 @@
         <v>0</v>
       </c>
       <c r="N38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O38">
         <f t="shared" si="0"/>
@@ -2234,10 +2234,10 @@
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -2255,10 +2255,10 @@
         <v>1</v>
       </c>
       <c r="I39">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J39">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -2270,7 +2270,7 @@
         <v>0</v>
       </c>
       <c r="N39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O39">
         <f t="shared" si="0"/>
@@ -2279,37 +2279,37 @@
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40">
+        <v>22</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40">
         <v>10</v>
       </c>
-      <c r="C40">
-        <v>7</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40">
-        <v>2</v>
-      </c>
-      <c r="I40">
-        <v>20</v>
-      </c>
       <c r="J40">
         <v>1</v>
       </c>
       <c r="K40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M40">
         <v>0</v>
@@ -2324,10 +2324,10 @@
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C41">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2342,25 +2342,25 @@
         <v>0</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I41">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41">
         <v>0</v>
       </c>
       <c r="N41">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O41">
         <f t="shared" si="0"/>
@@ -2369,10 +2369,10 @@
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -2381,19 +2381,19 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K42">
         <v>1</v>
@@ -2405,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="N42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O42">
         <f t="shared" si="0"/>
@@ -2414,16 +2414,16 @@
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -2432,25 +2432,25 @@
         <v>0</v>
       </c>
       <c r="H43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I43">
         <v>20</v>
       </c>
       <c r="J43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M43">
         <v>0</v>
       </c>
       <c r="N43">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O43">
         <f t="shared" si="0"/>
@@ -2459,31 +2459,31 @@
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C44">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44">
         <v>0</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I44">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K44">
         <v>1</v>
@@ -2495,40 +2495,40 @@
         <v>0</v>
       </c>
       <c r="N44">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O44">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="O44:O77" si="1">A44</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
         <v>10</v>
       </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>1</v>
-      </c>
-      <c r="I45">
-        <v>20</v>
-      </c>
       <c r="J45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K45">
         <v>0</v>
@@ -2540,25 +2540,25 @@
         <v>0</v>
       </c>
       <c r="N45">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="O45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -2570,31 +2570,31 @@
         <v>2</v>
       </c>
       <c r="I46">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J46">
         <v>2</v>
       </c>
       <c r="K46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M46">
         <v>0</v>
       </c>
       <c r="N46">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="O46">
-        <f t="shared" ref="O46:O80" si="1">A46</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C47">
         <v>2</v>
@@ -2615,10 +2615,10 @@
         <v>1</v>
       </c>
       <c r="I47">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K47">
         <v>0</v>
@@ -2630,7 +2630,7 @@
         <v>0</v>
       </c>
       <c r="N47">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="O47">
         <f t="shared" si="1"/>
@@ -2639,10 +2639,10 @@
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -2657,13 +2657,13 @@
         <v>0</v>
       </c>
       <c r="H48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I48">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="J48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K48">
         <v>0</v>
@@ -2675,7 +2675,7 @@
         <v>0</v>
       </c>
       <c r="N48">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O48">
         <f t="shared" si="1"/>
@@ -2684,10 +2684,10 @@
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2696,31 +2696,31 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I49">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="J49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M49">
         <v>0</v>
       </c>
       <c r="N49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O49">
         <f t="shared" si="1"/>
@@ -2729,10 +2729,10 @@
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -2747,25 +2747,25 @@
         <v>1</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I50">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="J50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M50">
         <v>0</v>
       </c>
       <c r="N50">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O50">
         <f t="shared" si="1"/>
@@ -2774,16 +2774,16 @@
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C51">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -2792,19 +2792,19 @@
         <v>0</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I51">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J51">
         <v>1</v>
       </c>
       <c r="K51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M51">
         <v>0</v>
@@ -2819,37 +2819,37 @@
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52">
+        <v>9</v>
+      </c>
+      <c r="C52">
         <v>8</v>
       </c>
-      <c r="C52">
-        <v>9</v>
-      </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52">
         <v>0</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52">
         <v>5</v>
       </c>
       <c r="J52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M52">
         <v>0</v>
@@ -2864,13 +2864,13 @@
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -2879,22 +2879,22 @@
         <v>0</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53">
         <v>3</v>
       </c>
       <c r="I53">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M53">
         <v>0</v>
@@ -2909,43 +2909,43 @@
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>3</v>
+      </c>
+      <c r="I54">
+        <v>5</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
         <v>7</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-      <c r="H54">
-        <v>3</v>
-      </c>
-      <c r="I54">
-        <v>15</v>
-      </c>
-      <c r="J54">
-        <v>1</v>
-      </c>
-      <c r="K54">
-        <v>1</v>
-      </c>
-      <c r="L54">
-        <v>0</v>
-      </c>
-      <c r="M54">
-        <v>0</v>
-      </c>
-      <c r="N54">
-        <v>6</v>
       </c>
       <c r="O54">
         <f t="shared" si="1"/>
@@ -2954,10 +2954,10 @@
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C55">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -2972,13 +2972,13 @@
         <v>0</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I55">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J55">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K55">
         <v>1</v>
@@ -2990,7 +2990,7 @@
         <v>0</v>
       </c>
       <c r="N55">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O55">
         <f t="shared" si="1"/>
@@ -2999,19 +2999,19 @@
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C56">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56">
         <v>0</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -3020,22 +3020,22 @@
         <v>3</v>
       </c>
       <c r="I56">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J56">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M56">
         <v>0</v>
       </c>
       <c r="N56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O56">
         <f t="shared" si="1"/>
@@ -3044,10 +3044,10 @@
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C57">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -3056,19 +3056,19 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57">
         <v>3</v>
       </c>
       <c r="I57">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K57">
         <v>1</v>
@@ -3080,7 +3080,7 @@
         <v>0</v>
       </c>
       <c r="N57">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="O57">
         <f t="shared" si="1"/>
@@ -3089,22 +3089,22 @@
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D58">
         <v>0</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F58">
         <v>0</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58">
         <v>2</v>
@@ -3125,7 +3125,7 @@
         <v>0</v>
       </c>
       <c r="N58">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O58">
         <f t="shared" si="1"/>
@@ -3134,10 +3134,10 @@
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C59">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -3152,13 +3152,13 @@
         <v>0</v>
       </c>
       <c r="H59">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I59">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K59">
         <v>1</v>
@@ -3170,7 +3170,7 @@
         <v>0</v>
       </c>
       <c r="N59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O59">
         <f t="shared" si="1"/>
@@ -3179,13 +3179,13 @@
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B60">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C60">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -3194,7 +3194,7 @@
         <v>0</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60">
         <v>3</v>
@@ -3203,19 +3203,19 @@
         <v>10</v>
       </c>
       <c r="J60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M60">
         <v>0</v>
       </c>
       <c r="N60">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="O60">
         <f t="shared" si="1"/>
@@ -3224,29 +3224,29 @@
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61">
+        <v>12</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
         <v>5</v>
       </c>
-      <c r="C61">
-        <v>9</v>
-      </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61">
-        <v>0</v>
-      </c>
-      <c r="G61">
-        <v>1</v>
-      </c>
-      <c r="H61">
-        <v>2</v>
-      </c>
-      <c r="I61">
-        <v>10</v>
-      </c>
       <c r="J61">
         <v>3</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>0</v>
       </c>
       <c r="N61">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O61">
         <f t="shared" si="1"/>
@@ -3269,43 +3269,43 @@
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C62">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I62">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J62">
         <v>2</v>
       </c>
       <c r="K62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M62">
         <v>0</v>
       </c>
       <c r="N62">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O62">
         <f t="shared" si="1"/>
@@ -3314,43 +3314,43 @@
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B63">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C63">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63">
         <v>0</v>
       </c>
       <c r="H63">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I63">
         <v>10</v>
       </c>
       <c r="J63">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M63">
         <v>0</v>
       </c>
       <c r="N63">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O63">
         <f t="shared" si="1"/>
@@ -3362,7 +3362,7 @@
         <v>4</v>
       </c>
       <c r="C64">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -3377,25 +3377,25 @@
         <v>0</v>
       </c>
       <c r="H64">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I64">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="J64">
         <v>3</v>
       </c>
       <c r="K64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M64">
         <v>0</v>
       </c>
       <c r="N64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O64">
         <f t="shared" si="1"/>
@@ -3404,43 +3404,43 @@
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B65">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D65">
         <v>0</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G65">
         <v>0</v>
       </c>
       <c r="H65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I65">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J65">
         <v>2</v>
       </c>
       <c r="K65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M65">
         <v>0</v>
       </c>
       <c r="N65">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O65">
         <f t="shared" si="1"/>
@@ -3449,10 +3449,10 @@
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C66">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -3461,19 +3461,19 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I66">
         <v>10</v>
       </c>
       <c r="J66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K66">
         <v>1</v>
@@ -3485,7 +3485,7 @@
         <v>0</v>
       </c>
       <c r="N66">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O66">
         <f t="shared" si="1"/>
@@ -3494,19 +3494,19 @@
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B67">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C67">
         <v>10</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -3521,16 +3521,16 @@
         <v>3</v>
       </c>
       <c r="K67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M67">
         <v>0</v>
       </c>
       <c r="N67">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O67">
         <f t="shared" si="1"/>
@@ -3539,25 +3539,25 @@
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B68">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C68">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D68">
         <v>0</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68">
         <v>0</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I68">
         <v>20</v>
@@ -3566,16 +3566,16 @@
         <v>2</v>
       </c>
       <c r="K68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M68">
         <v>0</v>
       </c>
       <c r="N68">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O68">
         <f t="shared" si="1"/>
@@ -3584,7 +3584,7 @@
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B69">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C69">
         <v>12</v>
@@ -3602,10 +3602,10 @@
         <v>1</v>
       </c>
       <c r="H69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I69">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J69">
         <v>2</v>
@@ -3620,7 +3620,7 @@
         <v>0</v>
       </c>
       <c r="N69">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O69">
         <f t="shared" si="1"/>
@@ -3629,7 +3629,7 @@
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B70">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C70">
         <v>10</v>
@@ -3641,31 +3641,31 @@
         <v>0</v>
       </c>
       <c r="F70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I70">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J70">
         <v>3</v>
       </c>
       <c r="K70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M70">
         <v>0</v>
       </c>
       <c r="N70">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="O70">
         <f t="shared" si="1"/>
@@ -3674,31 +3674,31 @@
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B71">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G71">
         <v>0</v>
       </c>
       <c r="H71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I71">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K71">
         <v>0</v>
@@ -3719,28 +3719,28 @@
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B72">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C72">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D72">
         <v>0</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F72">
         <v>0</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I72">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J72">
         <v>2</v>
@@ -3755,7 +3755,7 @@
         <v>0</v>
       </c>
       <c r="N72">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="O72">
         <f t="shared" si="1"/>
@@ -3764,10 +3764,10 @@
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B73">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C73">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -3782,10 +3782,10 @@
         <v>1</v>
       </c>
       <c r="H73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I73">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J73">
         <v>3</v>
@@ -3800,7 +3800,7 @@
         <v>0</v>
       </c>
       <c r="N73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O73">
         <f t="shared" si="1"/>
@@ -3809,19 +3809,19 @@
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B74">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C74">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
       <c r="F74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -3830,10 +3830,10 @@
         <v>1</v>
       </c>
       <c r="I74">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J74">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K74">
         <v>0</v>
@@ -3845,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="N74">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O74">
         <f t="shared" si="1"/>
@@ -3854,10 +3854,10 @@
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B75">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C75">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -3872,25 +3872,25 @@
         <v>0</v>
       </c>
       <c r="H75">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I75">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J75">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M75">
         <v>0</v>
       </c>
       <c r="N75">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="O75">
         <f t="shared" si="1"/>
@@ -3899,10 +3899,10 @@
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B76">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C76">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -3911,31 +3911,31 @@
         <v>0</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H76">
         <v>2</v>
       </c>
       <c r="I76">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="J76">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M76">
         <v>0</v>
       </c>
       <c r="N76">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O76">
         <f t="shared" si="1"/>
@@ -3944,7 +3944,7 @@
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B77">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C77">
         <v>11</v>
@@ -3965,159 +3965,24 @@
         <v>1</v>
       </c>
       <c r="I77">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J77">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M77">
         <v>0</v>
       </c>
       <c r="N77">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78">
-        <v>8</v>
-      </c>
-      <c r="C78">
-        <v>2</v>
-      </c>
-      <c r="D78">
-        <v>0</v>
-      </c>
-      <c r="E78">
-        <v>1</v>
-      </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-      <c r="G78">
-        <v>0</v>
-      </c>
-      <c r="H78">
-        <v>3</v>
-      </c>
-      <c r="I78">
-        <v>20</v>
-      </c>
-      <c r="J78">
-        <v>3</v>
-      </c>
-      <c r="K78">
-        <v>0</v>
-      </c>
-      <c r="L78">
-        <v>1</v>
-      </c>
-      <c r="M78">
-        <v>0</v>
-      </c>
-      <c r="N78">
-        <v>0</v>
-      </c>
-      <c r="O78">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79">
-        <v>15</v>
-      </c>
-      <c r="C79">
-        <v>1</v>
-      </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
-      <c r="E79">
-        <v>0</v>
-      </c>
-      <c r="F79">
-        <v>1</v>
-      </c>
-      <c r="G79">
-        <v>0</v>
-      </c>
-      <c r="H79">
-        <v>2</v>
-      </c>
-      <c r="I79">
-        <v>5</v>
-      </c>
-      <c r="J79">
-        <v>1</v>
-      </c>
-      <c r="K79">
-        <v>1</v>
-      </c>
-      <c r="L79">
-        <v>0</v>
-      </c>
-      <c r="M79">
-        <v>0</v>
-      </c>
-      <c r="N79">
-        <v>7</v>
-      </c>
-      <c r="O79">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80">
-        <v>13</v>
-      </c>
-      <c r="C80">
-        <v>11</v>
-      </c>
-      <c r="D80">
-        <v>1</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
-      <c r="F80">
-        <v>0</v>
-      </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-      <c r="H80">
-        <v>1</v>
-      </c>
-      <c r="I80">
-        <v>5</v>
-      </c>
-      <c r="J80">
-        <v>2</v>
-      </c>
-      <c r="K80">
-        <v>1</v>
-      </c>
-      <c r="L80">
-        <v>0</v>
-      </c>
-      <c r="M80">
-        <v>0</v>
-      </c>
-      <c r="N80">
-        <v>10</v>
-      </c>
-      <c r="O80">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>